<commit_message>
update alta lake data, remove stub vignettes
</commit_message>
<xml_diff>
--- a/data-raw/alta_lake_pb210.xlsx
+++ b/data-raw/alta_lake_pb210.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dewey/d/rdevel/pb210/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D451E24-2B56-FB4E-A983-E13D6CE0F0A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05794022-331C-2745-A951-4108B3FD6020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="3840" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{9AD30D51-AB46-5F49-9601-675826E02105}"/>
+    <workbookView xWindow="5500" yWindow="3840" windowWidth="27240" windowHeight="16440" xr2:uid="{9AD30D51-AB46-5F49-9601-675826E02105}"/>
   </bookViews>
   <sheets>
     <sheet name="drying" sheetId="1" r:id="rId1"/>
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB484FF2-D1E7-F049-ADDA-BF7437F14474}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2202,6 +2202,12 @@
       <c r="E33">
         <v>54.305686833300001</v>
       </c>
+      <c r="F33">
+        <v>23.893333340800002</v>
+      </c>
+      <c r="G33">
+        <v>0.7664887091218362</v>
+      </c>
       <c r="H33">
         <v>3.59</v>
       </c>
@@ -2218,7 +2224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B36552-11ED-E14A-8E5D-F19D1C590A56}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>